<commit_message>
19.02.2020 Mugdho Corporation Sales Details
</commit_message>
<xml_diff>
--- a/2020/January/All Details/30.01.2020/MC Bank Statement Jan'2020.xlsx
+++ b/2020/January/All Details/30.01.2020/MC Bank Statement Jan'2020.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\January\All Details\30.01.2020\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6015CE-5CCD-41BF-9E76-0FFE82DDEA30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="7" r:id="rId1"/>
     <sheet name="CAPITAL" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -232,9 +226,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1132,14 +1126,14 @@
     <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1616,12 +1610,12 @@
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Comma 2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Comma 2 3" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Comma 3" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 4" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 5" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 2" xfId="28"/>
+    <cellStyle name="Comma 2 2" xfId="29"/>
+    <cellStyle name="Comma 2 3" xfId="30"/>
+    <cellStyle name="Comma 3" xfId="31"/>
+    <cellStyle name="Comma 4" xfId="32"/>
+    <cellStyle name="Comma 5" xfId="33"/>
     <cellStyle name="Explanatory Text" xfId="34" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="35" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="36" builtinId="16" customBuiltin="1"/>
@@ -1632,15 +1626,15 @@
     <cellStyle name="Linked Cell" xfId="41" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="42" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 16" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 18" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 3" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 4" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Note 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Normal 16" xfId="43"/>
+    <cellStyle name="Normal 18" xfId="44"/>
+    <cellStyle name="Normal 2" xfId="45"/>
+    <cellStyle name="Normal 3" xfId="46"/>
+    <cellStyle name="Normal 4" xfId="47"/>
+    <cellStyle name="Note 2" xfId="48"/>
     <cellStyle name="Output" xfId="49" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Percent 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Percent 2" xfId="50"/>
+    <cellStyle name="Percent 3" xfId="51"/>
     <cellStyle name="Title" xfId="52" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="53" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="54" builtinId="11" customBuiltin="1"/>
@@ -1678,7 +1672,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1690,7 +1684,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1713,14 +1707,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1780,7 +1774,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1812,27 +1806,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1864,24 +1840,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2057,11 +2015,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2741,12 +2699,18 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="60"/>
-      <c r="B38" s="66"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="64"/>
+      <c r="B38" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="64">
+        <v>12000</v>
+      </c>
+      <c r="D38" s="64">
+        <v>0</v>
+      </c>
       <c r="E38" s="95">
         <f t="shared" ref="E38:E69" si="1">E37+C38-D38</f>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F38" s="56"/>
       <c r="G38" s="2"/>
@@ -2759,7 +2723,7 @@
       <c r="D39" s="64"/>
       <c r="E39" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F39" s="56"/>
       <c r="G39" s="2"/>
@@ -2772,7 +2736,7 @@
       <c r="D40" s="64"/>
       <c r="E40" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F40" s="56"/>
       <c r="G40" s="2"/>
@@ -2785,7 +2749,7 @@
       <c r="D41" s="64"/>
       <c r="E41" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F41" s="56"/>
       <c r="G41" s="2"/>
@@ -2798,7 +2762,7 @@
       <c r="D42" s="64"/>
       <c r="E42" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F42" s="56"/>
       <c r="G42" s="2"/>
@@ -2811,7 +2775,7 @@
       <c r="D43" s="64"/>
       <c r="E43" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F43" s="56"/>
       <c r="G43" s="2"/>
@@ -2824,7 +2788,7 @@
       <c r="D44" s="64"/>
       <c r="E44" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F44" s="56"/>
       <c r="G44" s="2"/>
@@ -2837,7 +2801,7 @@
       <c r="D45" s="64"/>
       <c r="E45" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F45" s="56"/>
       <c r="G45" s="2"/>
@@ -2850,7 +2814,7 @@
       <c r="D46" s="64"/>
       <c r="E46" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F46" s="56"/>
       <c r="G46" s="2"/>
@@ -2863,7 +2827,7 @@
       <c r="D47" s="64"/>
       <c r="E47" s="95">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F47" s="56"/>
       <c r="G47" s="2"/>
@@ -2876,7 +2840,7 @@
       <c r="D48" s="64"/>
       <c r="E48" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F48" s="56"/>
       <c r="G48" s="2"/>
@@ -2888,7 +2852,7 @@
       <c r="D49" s="64"/>
       <c r="E49" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F49" s="56"/>
       <c r="G49" s="2"/>
@@ -2900,7 +2864,7 @@
       <c r="D50" s="64"/>
       <c r="E50" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F50" s="56"/>
       <c r="G50" s="2"/>
@@ -2912,7 +2876,7 @@
       <c r="D51" s="64"/>
       <c r="E51" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F51" s="56"/>
       <c r="G51" s="2"/>
@@ -2924,7 +2888,7 @@
       <c r="D52" s="64"/>
       <c r="E52" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F52" s="56"/>
       <c r="G52" s="2"/>
@@ -2936,7 +2900,7 @@
       <c r="D53" s="64"/>
       <c r="E53" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F53" s="56"/>
       <c r="G53" s="2"/>
@@ -2948,7 +2912,7 @@
       <c r="D54" s="64"/>
       <c r="E54" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F54" s="56"/>
       <c r="G54" s="2"/>
@@ -2960,7 +2924,7 @@
       <c r="D55" s="64"/>
       <c r="E55" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F55" s="56"/>
       <c r="G55" s="2"/>
@@ -2971,7 +2935,7 @@
       <c r="D56" s="64"/>
       <c r="E56" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F56" s="56"/>
       <c r="G56" s="2"/>
@@ -2982,7 +2946,7 @@
       <c r="D57" s="64"/>
       <c r="E57" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F57" s="56"/>
       <c r="G57" s="2"/>
@@ -2993,7 +2957,7 @@
       <c r="D58" s="64"/>
       <c r="E58" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F58" s="56"/>
       <c r="G58" s="2"/>
@@ -3004,7 +2968,7 @@
       <c r="D59" s="64"/>
       <c r="E59" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F59" s="56"/>
       <c r="G59" s="2"/>
@@ -3015,7 +2979,7 @@
       <c r="D60" s="64"/>
       <c r="E60" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F60" s="56"/>
       <c r="G60" s="2"/>
@@ -3026,7 +2990,7 @@
       <c r="D61" s="64"/>
       <c r="E61" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F61" s="56"/>
       <c r="G61" s="2"/>
@@ -3037,7 +3001,7 @@
       <c r="D62" s="64"/>
       <c r="E62" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F62" s="56"/>
       <c r="G62" s="2"/>
@@ -3048,7 +3012,7 @@
       <c r="D63" s="64"/>
       <c r="E63" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F63" s="56"/>
       <c r="G63" s="2"/>
@@ -3059,7 +3023,7 @@
       <c r="D64" s="64"/>
       <c r="E64" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F64" s="56"/>
       <c r="G64" s="2"/>
@@ -3070,7 +3034,7 @@
       <c r="D65" s="64"/>
       <c r="E65" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F65" s="56"/>
       <c r="G65" s="2"/>
@@ -3081,7 +3045,7 @@
       <c r="D66" s="64"/>
       <c r="E66" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F66" s="56"/>
       <c r="G66" s="2"/>
@@ -3092,7 +3056,7 @@
       <c r="D67" s="64"/>
       <c r="E67" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F67" s="56"/>
       <c r="G67" s="2"/>
@@ -3103,7 +3067,7 @@
       <c r="D68" s="64"/>
       <c r="E68" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F68" s="56"/>
       <c r="G68" s="2"/>
@@ -3114,7 +3078,7 @@
       <c r="D69" s="64"/>
       <c r="E69" s="65">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F69" s="56"/>
       <c r="G69" s="2"/>
@@ -3125,7 +3089,7 @@
       <c r="D70" s="64"/>
       <c r="E70" s="65">
         <f t="shared" ref="E70:E82" si="2">E69+C70-D70</f>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F70" s="56"/>
       <c r="G70" s="2"/>
@@ -3136,7 +3100,7 @@
       <c r="D71" s="64"/>
       <c r="E71" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F71" s="56"/>
       <c r="G71" s="2"/>
@@ -3147,7 +3111,7 @@
       <c r="D72" s="64"/>
       <c r="E72" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F72" s="56"/>
       <c r="G72" s="2"/>
@@ -3158,7 +3122,7 @@
       <c r="D73" s="64"/>
       <c r="E73" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F73" s="56"/>
       <c r="G73" s="2"/>
@@ -3169,7 +3133,7 @@
       <c r="D74" s="64"/>
       <c r="E74" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F74" s="56"/>
       <c r="G74" s="2"/>
@@ -3180,7 +3144,7 @@
       <c r="D75" s="64"/>
       <c r="E75" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F75" s="58"/>
       <c r="G75" s="2"/>
@@ -3191,7 +3155,7 @@
       <c r="D76" s="64"/>
       <c r="E76" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F76" s="56"/>
       <c r="G76" s="2"/>
@@ -3202,7 +3166,7 @@
       <c r="D77" s="64"/>
       <c r="E77" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F77" s="56"/>
       <c r="G77" s="2"/>
@@ -3213,7 +3177,7 @@
       <c r="D78" s="64"/>
       <c r="E78" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F78" s="56"/>
       <c r="G78" s="2"/>
@@ -3224,7 +3188,7 @@
       <c r="D79" s="64"/>
       <c r="E79" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F79" s="56"/>
       <c r="G79" s="2"/>
@@ -3235,7 +3199,7 @@
       <c r="D80" s="64"/>
       <c r="E80" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F80" s="56"/>
       <c r="G80" s="2"/>
@@ -3246,7 +3210,7 @@
       <c r="D81" s="64"/>
       <c r="E81" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F81" s="56"/>
       <c r="G81" s="2"/>
@@ -3257,7 +3221,7 @@
       <c r="D82" s="64"/>
       <c r="E82" s="65">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>15000</v>
       </c>
       <c r="F82" s="56"/>
       <c r="G82" s="2"/>
@@ -3266,7 +3230,7 @@
       <c r="B83" s="72"/>
       <c r="C83" s="67">
         <f>SUM(C5:C72)</f>
-        <v>8502000</v>
+        <v>8514000</v>
       </c>
       <c r="D83" s="67">
         <f>SUM(D5:D77)</f>
@@ -3274,7 +3238,7 @@
       </c>
       <c r="E83" s="73">
         <f>E71+C83-D83</f>
-        <v>6000</v>
+        <v>30000</v>
       </c>
       <c r="F83" s="57"/>
       <c r="G83" s="2"/>
@@ -3296,13 +3260,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AK222"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>

</xml_diff>